<commit_message>
added additional dimensions to opafy dimensions table
</commit_message>
<xml_diff>
--- a/data/opafy_dimensions.xlsx
+++ b/data/opafy_dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenwh\Documents\Git\sentencing_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36981B62-FD30-4F70-8670-54F7C152974E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C1CC13-542C-424D-BDA4-049E6DD9EA8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7766E0A-5E4A-44A1-868B-E6ECEDE34DAB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7766E0A-5E4A-44A1-868B-E6ECEDE34DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="369">
   <si>
     <t>ZONE</t>
   </si>
@@ -1113,19 +1113,54 @@
     <t>SENTTOT0</t>
   </si>
   <si>
-    <t>SENTTOT1</t>
-  </si>
-  <si>
-    <t>SENTTOT2</t>
-  </si>
-  <si>
-    <t>SENTTOT3</t>
-  </si>
-  <si>
     <t>STA1_1</t>
   </si>
   <si>
     <t>STA2_1</t>
+  </si>
+  <si>
+    <t>The low end of the range of drug weight for first through nth drug types (DRUGTYP1-DRUGTYPX). This field is used when an exact amount was not specified in DRGAM1-DRGAMX but a range was provided. The weights are reported in several units of measure (UNIT1-UNITX).</t>
+  </si>
+  <si>
+    <t>Drug amount of the first through nth drug types (DRUGTYP1-DRUGTYPX) for which the defendant was held responsible. Often when weights are missing it is because both parties agreed to a Base Offense Level and the documents do not specify a corresponding drug amount. The weights are reported in several units of measure (UNIT1-UNITX), see WGT1- WGTX for the gram weight equivalency. For drug range amounts, see DAFROM1-DAFROMX and DATO1-DATOX.</t>
+  </si>
+  <si>
+    <t>The high end of the range of drug weight for first through nth drug types (DRUGTYP1-DRUGTYPX) when an exact amount was not specified in DRGAM1-DRGAMX. The weights are reported in several units of measure (UNIT1-UNITX).</t>
+  </si>
+  <si>
+    <t>Represents mandatory minimum sentence (in months) associated with 8§1324 (Immigration).</t>
+  </si>
+  <si>
+    <t>The dollar amount of loss for which the offender is held responsible. Amounts  are rounded off to the nearest whole dollar. Loss is often used in various economic crime guidelines to determine either the base offense level or levels of an SOC. Cases not involving dollar loss (ex. Drug cases) are coded as zero for the amount. Use variable NOCOMP to determine how many guideline computations are present in each case. All guideline variables available</t>
+  </si>
+  <si>
+    <t>Marital status of offender. This field is available FY1999-FY2003.</t>
+  </si>
+  <si>
+    <t>The difference in months between the guideline minimum (GLMIN) and the sentence length, including alternatives and probation as 0 months or incarceration (SENSPCAP). Only present for above and below range cases where the GLMIN is greater than 0 and less than life and the sentence is not life. Large values of GLMIN/MAX above sentencing table excluded from calcs. Field available FY2018-present.</t>
+  </si>
+  <si>
+    <t>The marijuana weight equivalency, in grams, of all the drug types coded. This variable is not missing if ANY of the individual marijuana equivalency weights are available (i.e., if the case involves two drugs and one type has weight available and one type does not have the weight available, then MWEIGHT will not be missing).</t>
+  </si>
+  <si>
+    <t>The marijuana weight equivalency, in grams, of the first through nth drug types (DRUGTYP1-DRUGTYPX)</t>
+  </si>
+  <si>
+    <t>Title, Section, and Subsection number of the UNIQUE statutes for each case generated from all of the statute fields (STAT1_1 thru STAT3_XX). Ex. If a case has a total of 5 counts involving 4 counts of 21:841 and one count of 18:924C then NWSTAT1 will be 21:841, NWSTAT2 will be 18:924C and NWSTAT3-X will be
+missing/inapplicable. These statute fields are not ordered; therefore, the first statute is not necessarily the most serious count. Use with NOUSTAT.</t>
+  </si>
+  <si>
+    <t>Primary offense type variable used in the FY2010 through FY2017 Sourcebook tables (this field replaces OFFTYPE2 although OFFTYPE2 is still available on the datafile through FY2017). This variable is based on the count of conviction with the highest statutory maximum (in case of a tie, the count with the highest statutory minimum is used). Note that since the primary offense type is derived from statutes of conviction it may not match up logically with the primary guideline (or any of the guidelines applied). See OFFTYPE2 for offense types used in USSC Sourcebook FY1999-FY2009. See OFFGUIDE for offense types used in USSC Sourcebook FY2018-present. Field available FY2010-FY2017.</t>
+  </si>
+  <si>
+    <t>The percent difference between the guideline minimum (GLMIN) and the sentence length, including alternatives and probation as 0 months or incarceration (SENSPCAP). Only present for above and below range cases where the GLMIN is greater than 0 and less than life and the sentence is not life. Large values of GLMIN/MAX above sentencing table excluded from calcs. Field available FY2018-present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigns cases to one of the 12 post-Booker reporting categories based on relationship between the sentence and guideline range and the reason(s) given
+for being outside of the range. </t>
+  </si>
+  <si>
+    <t>The total prison sentence (excluding months of alternative confinement), in months, with zeros (probation). Missing cases are set to "ꞏ". This field includes sentences of time imposed, time served, and §5G1.3 credit. See Appendix B in this codebook for more information about USSC sentencing variables. Field available FY1999-FY2017. See also SENTTCAP.</t>
   </si>
 </sst>
 </file>
@@ -1507,21 +1542,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C8BA2E-0235-47EA-927E-FA641C3982AB}">
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -1531,17 +1566,8 @@
       <c r="C1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -1551,17 +1577,8 @@
       <c r="C2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>152</v>
       </c>
@@ -1571,17 +1588,8 @@
       <c r="C3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>153</v>
       </c>
@@ -1591,11 +1599,8 @@
       <c r="C4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1605,11 +1610,8 @@
       <c r="C5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1619,11 +1621,8 @@
       <c r="C6" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1633,11 +1632,8 @@
       <c r="C7" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1647,11 +1643,8 @@
       <c r="C8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1661,11 +1654,8 @@
       <c r="C9" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>155</v>
       </c>
@@ -1675,11 +1665,8 @@
       <c r="C10" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>156</v>
       </c>
@@ -1689,11 +1676,8 @@
       <c r="C11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>157</v>
       </c>
@@ -1703,11 +1687,8 @@
       <c r="C12" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>158</v>
       </c>
@@ -1717,11 +1698,8 @@
       <c r="C13" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>159</v>
       </c>
@@ -1731,11 +1709,8 @@
       <c r="C14" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>160</v>
       </c>
@@ -1745,11 +1720,8 @@
       <c r="C15" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>161</v>
       </c>
@@ -1759,11 +1731,8 @@
       <c r="C16" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>162</v>
       </c>
@@ -1773,11 +1742,8 @@
       <c r="C17" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
@@ -1787,11 +1753,8 @@
       <c r="C18" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -1801,11 +1764,8 @@
       <c r="C19" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>165</v>
       </c>
@@ -1815,11 +1775,8 @@
       <c r="C20" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>154</v>
       </c>
@@ -1829,11 +1786,8 @@
       <c r="C21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1843,11 +1797,8 @@
       <c r="C22" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>166</v>
       </c>
@@ -1857,11 +1808,8 @@
       <c r="C23" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>167</v>
       </c>
@@ -1871,11 +1819,8 @@
       <c r="C24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1885,11 +1830,8 @@
       <c r="C25" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -1899,11 +1841,8 @@
       <c r="C26" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -1914,7 +1853,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1864,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -1936,7 +1875,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -1947,7 +1886,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -1958,7 +1897,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -3548,6 +3487,259 @@
       </c>
       <c r="C176" s="2" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A185" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A191" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A192" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding sas scripts and updated opafy dimensions
</commit_message>
<xml_diff>
--- a/data/opafy_dimensions.xlsx
+++ b/data/opafy_dimensions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenwh\Documents\Git\sentencing_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C1CC13-542C-424D-BDA4-049E6DD9EA8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037C0159-88D8-469B-88EF-0B9DCB166DFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7766E0A-5E4A-44A1-868B-E6ECEDE34DAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7766E0A-5E4A-44A1-868B-E6ECEDE34DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$202</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="371">
   <si>
     <t>ZONE</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>SEXACCB</t>
-  </si>
-  <si>
-    <t>SORFORM</t>
   </si>
   <si>
     <t>SUPRDUM</t>
@@ -966,9 +963,6 @@
   </si>
   <si>
     <t xml:space="preserve">Statutory minimum for each individual count of conviction. Use with variable NOCOUNT. See also STATMIN for overall statutory minimum for case. </t>
-  </si>
-  <si>
-    <t>REMOVE</t>
   </si>
   <si>
     <t>Title, Section, and Subsection number, respectively of the first statutes for each count of conviction. For example, STA1_123 is the 1st statute for the 123rd count of conviction. USSC records up to 3 statutes for each count. These statute fields are not ordered; therefore, the first
@@ -1080,9 +1074,6 @@
     <t>LOSS2</t>
   </si>
   <si>
-    <t>MARRIED</t>
-  </si>
-  <si>
     <t>MNTHDEPT</t>
   </si>
   <si>
@@ -1101,9 +1092,6 @@
     <t>NWSTAT2</t>
   </si>
   <si>
-    <t>OFFTYPSB</t>
-  </si>
-  <si>
     <t>PCNTDEPT</t>
   </si>
   <si>
@@ -1132,9 +1120,6 @@
   </si>
   <si>
     <t>The dollar amount of loss for which the offender is held responsible. Amounts  are rounded off to the nearest whole dollar. Loss is often used in various economic crime guidelines to determine either the base offense level or levels of an SOC. Cases not involving dollar loss (ex. Drug cases) are coded as zero for the amount. Use variable NOCOMP to determine how many guideline computations are present in each case. All guideline variables available</t>
-  </si>
-  <si>
-    <t>Marital status of offender. This field is available FY1999-FY2003.</t>
   </si>
   <si>
     <t>The difference in months between the guideline minimum (GLMIN) and the sentence length, including alternatives and probation as 0 months or incarceration (SENSPCAP). Only present for above and below range cases where the GLMIN is greater than 0 and less than life and the sentence is not life. Large values of GLMIN/MAX above sentencing table excluded from calcs. Field available FY2018-present.</t>
@@ -1150,9 +1135,6 @@
 missing/inapplicable. These statute fields are not ordered; therefore, the first statute is not necessarily the most serious count. Use with NOUSTAT.</t>
   </si>
   <si>
-    <t>Primary offense type variable used in the FY2010 through FY2017 Sourcebook tables (this field replaces OFFTYPE2 although OFFTYPE2 is still available on the datafile through FY2017). This variable is based on the count of conviction with the highest statutory maximum (in case of a tie, the count with the highest statutory minimum is used). Note that since the primary offense type is derived from statutes of conviction it may not match up logically with the primary guideline (or any of the guidelines applied). See OFFTYPE2 for offense types used in USSC Sourcebook FY1999-FY2009. See OFFGUIDE for offense types used in USSC Sourcebook FY2018-present. Field available FY2010-FY2017.</t>
-  </si>
-  <si>
     <t>The percent difference between the guideline minimum (GLMIN) and the sentence length, including alternatives and probation as 0 months or incarceration (SENSPCAP). Only present for above and below range cases where the GLMIN is greater than 0 and less than life and the sentence is not life. Large values of GLMIN/MAX above sentencing table excluded from calcs. Field available FY2018-present.</t>
   </si>
   <si>
@@ -1161,6 +1143,30 @@
   </si>
   <si>
     <t>The total prison sentence (excluding months of alternative confinement), in months, with zeros (probation). Missing cases are set to "ꞏ". This field includes sentences of time imposed, time served, and §5G1.3 credit. See Appendix B in this codebook for more information about USSC sentencing variables. Field available FY1999-FY2017. See also SENTTCAP.</t>
+  </si>
+  <si>
+    <t>ADJ_D1</t>
+  </si>
+  <si>
+    <t>ADJ_D2</t>
+  </si>
+  <si>
+    <t>ADJ_D3</t>
+  </si>
+  <si>
+    <t>Indicates whether offender caused bodily injury</t>
+  </si>
+  <si>
+    <t>ADJ_E1</t>
+  </si>
+  <si>
+    <t>ADJ_E2</t>
+  </si>
+  <si>
+    <t>ADJ_E3</t>
+  </si>
+  <si>
+    <t>Indicates whether offender participated in kidnapping</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1186,6 +1192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1217,7 +1229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1226,6 +1238,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1542,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C8BA2E-0235-47EA-927E-FA641C3982AB}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,46 +1576,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1605,10 +1623,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1616,10 +1634,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1627,10 +1645,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1638,10 +1656,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -1649,142 +1667,142 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1792,32 +1810,32 @@
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1825,10 +1843,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1836,10 +1854,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1847,10 +1865,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1858,10 +1876,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -1869,1883 +1887,1919 @@
         <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C31" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="C32" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>203</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="C47" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="C49" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="60" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="C60" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="C63" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="B64" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="C64" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="B65" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="B66" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B73" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>223</v>
+      <c r="C76" s="4" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>247</v>
+        <v>354</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>63</v>
+        <v>338</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>252</v>
+        <v>355</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>64</v>
+        <v>339</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>253</v>
+        <v>355</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>72</v>
+        <v>340</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>262</v>
+        <v>356</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>81</v>
+        <v>341</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>273</v>
+        <v>357</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>80</v>
+        <v>342</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>272</v>
+        <v>358</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>82</v>
+        <v>343</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>274</v>
+        <v>358</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>282</v>
+        <v>204</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>89</v>
+        <v>344</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>285</v>
+        <v>359</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>90</v>
+        <v>345</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>286</v>
+        <v>359</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>93</v>
+        <v>346</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>290</v>
+        <v>360</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C136" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A139" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="C139" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A151" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A160" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B149" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A151" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="B163" s="3" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>10</v>
+        <v>349</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>172</v>
+        <v>350</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>353</v>
+        <v>148</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>354</v>
+        <v>102</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
-        <v>333</v>
+        <v>103</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>334</v>
+        <v>147</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>355</v>
+        <v>318</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>335</v>
+        <v>104</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>336</v>
+        <v>105</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
-        <v>337</v>
+        <v>106</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>338</v>
+        <v>107</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>339</v>
+        <v>108</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>340</v>
+        <v>109</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
-        <v>341</v>
+        <v>170</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>359</v>
+        <v>322</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>270</v>
+        <v>178</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
-        <v>342</v>
+        <v>10</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>343</v>
+        <v>171</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>344</v>
+        <v>110</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>362</v>
+        <v>325</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>345</v>
+        <v>112</v>
       </c>
       <c r="B192" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A193" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A194" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A196" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>366</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="B198" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A199" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B199" s="3" t="s">
+      <c r="B200" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>223</v>
+      <c r="B201" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D176" xr:uid="{F391D5E2-F58A-4978-9340-6BAC3823A52B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A176">
-    <sortCondition ref="A1:A176"/>
+  <autoFilter ref="A1:D202" xr:uid="{F391D5E2-F58A-4978-9340-6BAC3823A52B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C196">
+    <sortCondition ref="A2:A196"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>